<commit_message>
Alternative way to create large array brought up
</commit_message>
<xml_diff>
--- a/Excel_Challenge_419 - Reverse Divisible & Not Palindromes.xlsx
+++ b/Excel_Challenge_419 - Reverse Divisible & Not Palindromes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{832C72EE-435A-4EB5-A434-DE4298D6F6A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C2CC4E-C826-48DF-981B-136004F00BB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Expected Answer</t>
   </si>
@@ -82,12 +82,15 @@
   <si>
     <t>There are only 11 numbers here. The problem states 12.</t>
   </si>
+  <si>
+    <t>I should be able to use Makearray here instead of the dual SEQUENCE approach.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,6 +116,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -144,12 +154,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -624,8 +635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -928,6 +939,11 @@
         <v>1</v>
       </c>
     </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H14" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G16" t="str" cm="1">
         <f t="array" ref="G16">_xlfn.REDUCE("",_xlfn.SEQUENCE(5*10^5)+_xlfn.SEQUENCE(1,44,0,500000),_xlfn.LAMBDA(_xlpm.x,_xlpm.y,IF(testIt(_xlpm.y),_xlpm.x&amp;"|"&amp;_xlpm.y,_xlpm.x)))</f>

</xml_diff>